<commit_message>
Timing Chart fixed, stylesheet moved and a printing style sheet created.
Timing chart functionality restored, style sheets moved. a printing style sheet created (I don't want the form when I'm cooking)
</commit_message>
<xml_diff>
--- a/Alterations to make.xlsx
+++ b/Alterations to make.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\roastdinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D97C6EA-3C6F-4F0D-A622-6B82B16498BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489C6012-896A-4701-A6A9-4782F1C046B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30480" yWindow="23805" windowWidth="29070" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Foods To Add</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Mash</t>
   </si>
   <si>
-    <t>Split out Green Vegtables?</t>
-  </si>
-  <si>
     <t>Gravy from Meat Juices</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Oven Size Estimate</t>
   </si>
   <si>
-    <t>Move CCS to another File and tag elements</t>
-  </si>
-  <si>
     <t>Meet Thermometer suggestion</t>
   </si>
   <si>
@@ -81,13 +75,13 @@
     <t>Serving estimate</t>
   </si>
   <si>
-    <t>Timing chart printing</t>
-  </si>
-  <si>
     <t>Import Ingredients from other file</t>
   </si>
   <si>
     <t>Filter More Complex Sauces</t>
+  </si>
+  <si>
+    <t>Clear Button</t>
   </si>
 </sst>
 </file>
@@ -405,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F23"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F5" sqref="E5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,11 +417,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
@@ -438,10 +427,10 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
         <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -454,60 +443,55 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stylistic Changes and UI stubs for future development
Added new UI elements moving settings to the top and starting the process of adding filters and further hidden functionality.
</commit_message>
<xml_diff>
--- a/Alterations to make.xlsx
+++ b/Alterations to make.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\roastdinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489C6012-896A-4701-A6A9-4782F1C046B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A38EA6E-D7E8-4E01-8093-613599B4F2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30480" yWindow="23805" windowWidth="29070" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33375" yWindow="6810" windowWidth="22425" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Foods To Add</t>
   </si>
@@ -51,24 +51,15 @@
     <t xml:space="preserve">Filters </t>
   </si>
   <si>
-    <t>Tradition vs other stuff</t>
-  </si>
-  <si>
     <t>Managing Time Pinch points.</t>
   </si>
   <si>
     <t>Oven Size Estimate</t>
   </si>
   <si>
-    <t>Meet Thermometer suggestion</t>
-  </si>
-  <si>
     <t>Contential Meat Advice</t>
   </si>
   <si>
-    <t>Veg End Points</t>
-  </si>
-  <si>
     <t>Ingrediant calculator</t>
   </si>
   <si>
@@ -78,18 +69,26 @@
     <t>Import Ingredients from other file</t>
   </si>
   <si>
-    <t>Filter More Complex Sauces</t>
-  </si>
-  <si>
     <t>Clear Button</t>
+  </si>
+  <si>
+    <t>Complex vs Traditional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,102 +399,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="E5:F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
       <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
         <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>